<commit_message>
Update and fill some values.
</commit_message>
<xml_diff>
--- a/solventSelectionTool_table.xlsx
+++ b/solventSelectionTool_table.xlsx
@@ -18,7 +18,6 @@
     <sheet name="Data excluded" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3567,7 +3566,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3891,7 +3897,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3902,8 +3908,8 @@
     <col min="4" max="4" width="10.54296875" style="12" customWidth="1"/>
     <col min="5" max="5" width="10.26953125" style="21" customWidth="1"/>
     <col min="6" max="6" width="7.81640625" style="134" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="14" customWidth="1"/>
-    <col min="8" max="9" width="8.7265625" style="141" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="14" customWidth="1"/>
+    <col min="8" max="9" width="8.81640625" style="141" customWidth="1"/>
     <col min="10" max="10" width="9.1796875" style="47"/>
     <col min="11" max="12" width="9.1796875" style="10"/>
     <col min="13" max="13" width="9.1796875" style="115"/>
@@ -6408,7 +6414,9 @@
       <c r="H38" s="48">
         <v>3.0910000000000002</v>
       </c>
-      <c r="I38" s="14"/>
+      <c r="I38" s="14">
+        <v>42</v>
+      </c>
       <c r="J38" s="47">
         <v>1</v>
       </c>
@@ -7388,7 +7396,9 @@
       <c r="H53" s="48">
         <v>1.86</v>
       </c>
-      <c r="I53" s="14"/>
+      <c r="I53" s="14">
+        <v>32.299999999999997</v>
+      </c>
       <c r="U53" s="46" t="s">
         <v>312</v>
       </c>
@@ -7421,7 +7431,9 @@
       <c r="H54" s="48">
         <v>1.7589999999999999</v>
       </c>
-      <c r="I54" s="14"/>
+      <c r="I54" s="14">
+        <v>32.1</v>
+      </c>
       <c r="U54" s="46" t="s">
         <v>863</v>
       </c>
@@ -7554,7 +7566,9 @@
       <c r="H57" s="48">
         <v>1.79</v>
       </c>
-      <c r="I57" s="14"/>
+      <c r="I57" s="14">
+        <v>35.799999999999997</v>
+      </c>
       <c r="U57" s="46" t="s">
         <v>867</v>
       </c>
@@ -7620,7 +7634,7 @@
         <v>246</v>
       </c>
       <c r="H59" s="48">
-        <v>0.3</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="I59" s="14">
         <v>48.5</v>
@@ -7758,7 +7772,9 @@
       <c r="H61" s="48">
         <v>1.089</v>
       </c>
-      <c r="I61" s="14"/>
+      <c r="I61" s="14">
+        <v>25.6</v>
+      </c>
       <c r="J61" s="47">
         <v>4</v>
       </c>
@@ -8020,7 +8036,7 @@
         <v>10</v>
       </c>
       <c r="G65" s="14">
-        <v>110</v>
+        <v>227</v>
       </c>
       <c r="H65" s="48">
         <v>3.03</v>
@@ -8226,7 +8242,9 @@
       <c r="H68" s="48">
         <v>2.92</v>
       </c>
-      <c r="I68" s="14"/>
+      <c r="I68" s="14">
+        <v>32.1</v>
+      </c>
       <c r="J68" s="47">
         <v>4</v>
       </c>
@@ -8686,7 +8704,7 @@
         <v>54</v>
       </c>
       <c r="H75" s="48">
-        <v>11.167</v>
+        <v>0.4</v>
       </c>
       <c r="I75" s="14">
         <v>24</v>
@@ -9017,7 +9035,7 @@
         <v>2.58</v>
       </c>
       <c r="I80" s="14">
-        <v>20</v>
+        <v>32.1</v>
       </c>
       <c r="J80" s="47">
         <v>5</v>
@@ -9945,12 +9963,14 @@
         <v>17</v>
       </c>
       <c r="G94" s="14">
-        <v>122</v>
+        <v>217</v>
       </c>
       <c r="H94" s="48">
         <v>36.9</v>
       </c>
-      <c r="I94" s="14"/>
+      <c r="I94" s="14">
+        <v>49.8</v>
+      </c>
       <c r="J94" s="47">
         <v>3</v>
       </c>
@@ -10410,7 +10430,9 @@
       <c r="H101" s="48">
         <v>0.437</v>
       </c>
-      <c r="I101" s="14"/>
+      <c r="I101" s="14">
+        <v>23.6</v>
+      </c>
       <c r="J101" s="47">
         <v>5</v>
       </c>
@@ -10746,7 +10768,7 @@
         <v>0.68500000000000005</v>
       </c>
       <c r="I106" s="14">
-        <v>14.5</v>
+        <v>23</v>
       </c>
       <c r="J106" s="47">
         <v>8</v>
@@ -11014,7 +11036,9 @@
       <c r="H110" s="48">
         <v>11.46</v>
       </c>
-      <c r="I110" s="14"/>
+      <c r="I110" s="14">
+        <v>28.3</v>
+      </c>
       <c r="J110" s="47">
         <v>9</v>
       </c>
@@ -11149,7 +11173,7 @@
         <v>0.92</v>
       </c>
       <c r="I112" s="14">
-        <v>12</v>
+        <v>24.7</v>
       </c>
       <c r="J112" s="47">
         <v>7</v>
@@ -11542,7 +11566,7 @@
         <v>188</v>
       </c>
       <c r="H118" s="48">
-        <v>0.58099999999999996</v>
+        <v>42</v>
       </c>
       <c r="I118" s="14">
         <v>40.099999999999994</v>
@@ -12215,7 +12239,9 @@
       <c r="H128" s="48">
         <v>1.5</v>
       </c>
-      <c r="I128" s="14"/>
+      <c r="I128" s="14">
+        <v>30.2</v>
+      </c>
       <c r="J128" s="47">
         <v>3</v>
       </c>
@@ -12346,7 +12372,9 @@
       <c r="H130" s="48">
         <v>24</v>
       </c>
-      <c r="I130" s="14"/>
+      <c r="I130" s="14">
+        <v>36.5</v>
+      </c>
       <c r="J130" s="47">
         <v>5</v>
       </c>
@@ -12474,7 +12502,9 @@
         <v>83</v>
       </c>
       <c r="H132" s="48"/>
-      <c r="I132" s="14"/>
+      <c r="I132" s="14">
+        <v>44.7</v>
+      </c>
       <c r="J132" s="47">
         <v>4</v>
       </c>

</xml_diff>